<commit_message>
first draft of analysis write-up.
</commit_message>
<xml_diff>
--- a/Resources/Data_Frames_Simple_vs_Wgt_Averages.xlsx
+++ b/Resources/Data_Frames_Simple_vs_Wgt_Averages.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignacioguerra/Desktop/DATA_BOOTCAMP_WORK/MODULE_4/School_District_Analysis/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9AA19BF-CEC0-C841-895D-A3A7C0CDBF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB85DDD-5F2A-6D42-B08A-F449223BBEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="4060" windowWidth="24160" windowHeight="13300" xr2:uid="{DF40913C-A240-FC47-92AA-8B89F110E5A1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16700" activeTab="1" xr2:uid="{DF40913C-A240-FC47-92AA-8B89F110E5A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="School Type" sheetId="1" r:id="rId1"/>
+    <sheet name="By School Type" sheetId="1" r:id="rId1"/>
+    <sheet name="By Spending Ranges" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="37">
   <si>
     <t>Bailey High School</t>
   </si>
@@ -87,7 +89,64 @@
     <t>Wright High School</t>
   </si>
   <si>
-    <t>AVERAGE FOR DISTRICT SCHOOLS</t>
+    <t>&lt;$584</t>
+  </si>
+  <si>
+    <t>Medium (1000-2000)</t>
+  </si>
+  <si>
+    <t>$585-629</t>
+  </si>
+  <si>
+    <t>$630-644</t>
+  </si>
+  <si>
+    <t>Large (2000-5000)</t>
+  </si>
+  <si>
+    <t>$645-675</t>
+  </si>
+  <si>
+    <t>Small (&lt;1000)</t>
+  </si>
+  <si>
+    <t>WEIGHTED AVERAGE</t>
+  </si>
+  <si>
+    <t>School Type</t>
+  </si>
+  <si>
+    <t>Total Students</t>
+  </si>
+  <si>
+    <t>Total School Budget</t>
+  </si>
+  <si>
+    <t>Per Student Budget</t>
+  </si>
+  <si>
+    <t>Average Math Score</t>
+  </si>
+  <si>
+    <t>Average Reading Score</t>
+  </si>
+  <si>
+    <t>% Passing Math</t>
+  </si>
+  <si>
+    <t>% Passing Reading</t>
+  </si>
+  <si>
+    <t>% Overall Passing</t>
+  </si>
+  <si>
+    <t>Spending Ranges (Per Student)</t>
+  </si>
+  <si>
+    <t>School Size</t>
+  </si>
+  <si>
+    <t>SIMPLE AVERAGE</t>
   </si>
 </sst>
 </file>
@@ -97,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +189,14 @@
       <color theme="1"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -170,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -178,11 +245,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -200,6 +276,20 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,19 +604,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46467209-055F-C141-9356-109201465BC0}">
-  <dimension ref="C3:L23"/>
+  <dimension ref="C2:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:14" s="16" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
@@ -557,8 +691,14 @@
       <c r="L3" s="2">
         <v>91.334768999999994</v>
       </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
@@ -589,8 +729,14 @@
       <c r="L4" s="2">
         <v>90.599455000000006</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
@@ -621,8 +767,14 @@
       <c r="L5" s="2">
         <v>89.227165999999997</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
@@ -653,8 +805,14 @@
       <c r="L6" s="2">
         <v>90.540541000000005</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
@@ -685,8 +843,14 @@
       <c r="L7" s="2">
         <v>89.892106999999996</v>
       </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
@@ -717,8 +881,14 @@
       <c r="L8" s="2">
         <v>90.630324000000002</v>
       </c>
-    </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>15</v>
       </c>
@@ -749,8 +919,14 @@
       <c r="L9" s="2">
         <v>90.582566999999997</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
@@ -781,8 +957,14 @@
       <c r="L10" s="2">
         <v>90.333332999999996</v>
       </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,8 +995,14 @@
       <c r="L11" s="13">
         <v>54.642282999999999</v>
       </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
@@ -845,8 +1033,14 @@
       <c r="L12" s="13">
         <v>53.204476</v>
       </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
@@ -877,8 +1071,14 @@
       <c r="L13" s="13">
         <v>54.289887</v>
       </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
@@ -909,8 +1109,14 @@
       <c r="L14" s="13">
         <v>53.527507999999997</v>
       </c>
-    </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
@@ -941,8 +1147,14 @@
       <c r="L15" s="13">
         <v>53.513883999999997</v>
       </c>
-    </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
@@ -973,8 +1185,14 @@
       <c r="L16" s="13">
         <v>53.539172000000001</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1005,12 +1223,18 @@
       <c r="L17" s="13">
         <v>52.988247000000001</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="M17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="F19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H19" s="6">
@@ -1034,77 +1258,91 @@
         <v>53.672208142857144</v>
       </c>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="G20" t="s">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F20" s="19"/>
+      <c r="G20" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="19">
         <f>AVERAGE(H3:H10)</f>
         <v>83.465425625000009</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="19">
         <f>AVERAGE(I3:I10)</f>
         <v>83.902314750000002</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="19">
         <f>AVERAGE(J3:J10)</f>
         <v>93.610020000000006</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="19">
         <f>AVERAGE(K3:K10)</f>
         <v>96.550223125000002</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="19">
         <f>AVERAGE(L3:L10)</f>
         <v>90.392532750000015</v>
       </c>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="G22" t="s">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F22" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="19">
         <f>(H11*$E11+H12*$E12+H13*$E13+H14*$E14+H15*$E15+H16*$E16+H17*$E17)/SUM($E11:$E17)</f>
         <v>76.9870255617586</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="19">
         <f t="shared" ref="I22:L22" si="1">(I11*$E11+I12*$E12+I13*$E13+I14*$E14+I15*$E15+I16*$E16+I17*$E17)/SUM($E11:$E17)</f>
         <v>80.962485259934752</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="19">
         <f t="shared" si="1"/>
         <v>66.518386846048344</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="19">
         <f t="shared" si="1"/>
         <v>80.905249140384043</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="19">
         <f t="shared" si="1"/>
         <v>53.695877716414593</v>
       </c>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="G23" t="s">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="19">
         <f>(H3*$E3+H4*$E4+H5*$E5+H6*$E6+H7*$E7+H8*($E8-461)+H9*$E9+H10*$E10)/(SUM($E3:$E10)-461)</f>
         <v>83.398960411233276</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="19">
         <f t="shared" ref="I23:L23" si="2">(I3*$E3+I4*$E4+I5*$E5+I6*$E6+I7*$E7+I8*($E8-461)+I9*$E9+I10*$E10)/(SUM($E3:$E10)-461)</f>
         <v>83.909656538481201</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="19">
         <f t="shared" si="2"/>
         <v>93.710048675019181</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="19">
         <f t="shared" si="2"/>
         <v>96.59081229199694</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="19">
         <f t="shared" si="2"/>
         <v>90.513935202420512</v>
       </c>
@@ -1116,4 +1354,826 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235F173A-F0EF-6644-9AFD-0376C8AE632D}">
+  <dimension ref="C2:N27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:14" s="16" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1858</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1081356</v>
+      </c>
+      <c r="G3" s="3">
+        <v>582</v>
+      </c>
+      <c r="H3" s="2">
+        <v>83.061895000000007</v>
+      </c>
+      <c r="I3" s="2">
+        <v>83.97578</v>
+      </c>
+      <c r="J3" s="2">
+        <v>94.133476999999999</v>
+      </c>
+      <c r="K3" s="2">
+        <v>97.039828</v>
+      </c>
+      <c r="L3" s="2">
+        <v>91.334768999999994</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>427</v>
+      </c>
+      <c r="F4" s="3">
+        <v>248087</v>
+      </c>
+      <c r="G4" s="3">
+        <v>581</v>
+      </c>
+      <c r="H4" s="2">
+        <v>83.803279000000003</v>
+      </c>
+      <c r="I4" s="2">
+        <v>83.814988</v>
+      </c>
+      <c r="J4" s="2">
+        <v>92.505854999999997</v>
+      </c>
+      <c r="K4" s="2">
+        <v>96.252927</v>
+      </c>
+      <c r="L4" s="2">
+        <v>89.227165999999997</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2283</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1319574</v>
+      </c>
+      <c r="G5" s="3">
+        <v>578</v>
+      </c>
+      <c r="H5" s="2">
+        <v>83.274201000000005</v>
+      </c>
+      <c r="I5" s="2">
+        <v>83.989487999999994</v>
+      </c>
+      <c r="J5" s="2">
+        <v>93.867717999999996</v>
+      </c>
+      <c r="K5" s="2">
+        <v>96.539641000000003</v>
+      </c>
+      <c r="L5" s="2">
+        <v>90.582566999999997</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1049400</v>
+      </c>
+      <c r="G6" s="3">
+        <v>583</v>
+      </c>
+      <c r="H6" s="2">
+        <v>83.682221999999996</v>
+      </c>
+      <c r="I6" s="2">
+        <v>83.954999999999998</v>
+      </c>
+      <c r="J6" s="2">
+        <v>93.333332999999996</v>
+      </c>
+      <c r="K6" s="2">
+        <v>96.611110999999994</v>
+      </c>
+      <c r="L6" s="2">
+        <v>90.333332999999996</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1468</v>
+      </c>
+      <c r="F7" s="3">
+        <v>917500</v>
+      </c>
+      <c r="G7" s="3">
+        <v>625</v>
+      </c>
+      <c r="H7" s="2">
+        <v>83.351499000000004</v>
+      </c>
+      <c r="I7" s="2">
+        <v>83.816756999999996</v>
+      </c>
+      <c r="J7" s="2">
+        <v>93.392370999999997</v>
+      </c>
+      <c r="K7" s="2">
+        <v>97.138964999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>90.599455000000006</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>962</v>
+      </c>
+      <c r="F8" s="3">
+        <v>585858</v>
+      </c>
+      <c r="G8" s="3">
+        <v>609</v>
+      </c>
+      <c r="H8" s="2">
+        <v>83.839917</v>
+      </c>
+      <c r="I8" s="2">
+        <v>84.044698999999994</v>
+      </c>
+      <c r="J8" s="2">
+        <v>94.594594999999998</v>
+      </c>
+      <c r="K8" s="2">
+        <v>95.945946000000006</v>
+      </c>
+      <c r="L8" s="2">
+        <v>90.540541000000005</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1761</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1056600</v>
+      </c>
+      <c r="G9" s="3">
+        <v>600</v>
+      </c>
+      <c r="H9" s="2">
+        <v>83.359454999999997</v>
+      </c>
+      <c r="I9" s="2">
+        <v>83.725724</v>
+      </c>
+      <c r="J9" s="2">
+        <v>93.867120999999997</v>
+      </c>
+      <c r="K9" s="2">
+        <v>95.854628000000005</v>
+      </c>
+      <c r="L9" s="2">
+        <v>89.892106999999996</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4976</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3124928</v>
+      </c>
+      <c r="G10" s="3">
+        <v>628</v>
+      </c>
+      <c r="H10" s="20">
+        <v>77.048432000000005</v>
+      </c>
+      <c r="I10" s="20">
+        <v>81.033963</v>
+      </c>
+      <c r="J10" s="20">
+        <v>66.680064000000002</v>
+      </c>
+      <c r="K10" s="20">
+        <v>81.933279999999996</v>
+      </c>
+      <c r="L10" s="20">
+        <v>54.642282999999999</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1635</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1043130</v>
+      </c>
+      <c r="G11" s="3">
+        <v>638</v>
+      </c>
+      <c r="H11" s="20">
+        <v>83.350937000000002</v>
+      </c>
+      <c r="I11" s="20">
+        <v>83.896082000000007</v>
+      </c>
+      <c r="J11" s="20">
+        <v>93.185689999999994</v>
+      </c>
+      <c r="K11" s="20">
+        <v>97.018738999999997</v>
+      </c>
+      <c r="L11" s="20">
+        <v>90.630324000000002</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2949</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1884411</v>
+      </c>
+      <c r="G12" s="3">
+        <v>639</v>
+      </c>
+      <c r="H12" s="20">
+        <v>76.711766999999995</v>
+      </c>
+      <c r="I12" s="20">
+        <v>81.158019999999993</v>
+      </c>
+      <c r="J12" s="20">
+        <v>65.988471000000004</v>
+      </c>
+      <c r="K12" s="20">
+        <v>80.739233999999996</v>
+      </c>
+      <c r="L12" s="20">
+        <v>53.204476</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2739</v>
+      </c>
+      <c r="F13" s="3">
+        <v>1763916</v>
+      </c>
+      <c r="G13" s="3">
+        <v>644</v>
+      </c>
+      <c r="H13" s="20">
+        <v>77.102592000000001</v>
+      </c>
+      <c r="I13" s="20">
+        <v>80.746257999999997</v>
+      </c>
+      <c r="J13" s="20">
+        <v>68.309601999999998</v>
+      </c>
+      <c r="K13" s="20">
+        <v>79.299014</v>
+      </c>
+      <c r="L13" s="20">
+        <v>54.289887</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3999</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2547363</v>
+      </c>
+      <c r="G14" s="3">
+        <v>637</v>
+      </c>
+      <c r="H14" s="20">
+        <v>76.842710999999994</v>
+      </c>
+      <c r="I14" s="20">
+        <v>80.744686000000002</v>
+      </c>
+      <c r="J14" s="20">
+        <v>66.366591999999997</v>
+      </c>
+      <c r="K14" s="20">
+        <v>80.220055000000002</v>
+      </c>
+      <c r="L14" s="20">
+        <v>52.988247000000001</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>4635</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3022020</v>
+      </c>
+      <c r="G15" s="3">
+        <v>652</v>
+      </c>
+      <c r="H15" s="20">
+        <v>77.289751999999993</v>
+      </c>
+      <c r="I15" s="20">
+        <v>80.934411999999995</v>
+      </c>
+      <c r="J15" s="20">
+        <v>66.752966999999998</v>
+      </c>
+      <c r="K15" s="20">
+        <v>80.862999000000002</v>
+      </c>
+      <c r="L15" s="20">
+        <v>53.527507999999997</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2917</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1910635</v>
+      </c>
+      <c r="G16" s="3">
+        <v>655</v>
+      </c>
+      <c r="H16" s="20">
+        <v>76.629413999999997</v>
+      </c>
+      <c r="I16" s="20">
+        <v>81.182721999999998</v>
+      </c>
+      <c r="J16" s="20">
+        <v>65.683921999999995</v>
+      </c>
+      <c r="K16" s="20">
+        <v>81.316421000000005</v>
+      </c>
+      <c r="L16" s="20">
+        <v>53.513883999999997</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4761</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3094650</v>
+      </c>
+      <c r="G17" s="3">
+        <v>650</v>
+      </c>
+      <c r="H17" s="20">
+        <v>77.072463999999997</v>
+      </c>
+      <c r="I17" s="20">
+        <v>80.966393999999994</v>
+      </c>
+      <c r="J17" s="20">
+        <v>66.057551000000004</v>
+      </c>
+      <c r="K17" s="20">
+        <v>81.222431999999998</v>
+      </c>
+      <c r="L17" s="20">
+        <v>53.539172000000001</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="22">
+        <f>AVERAGE(H3:H6)</f>
+        <v>83.455399249999999</v>
+      </c>
+      <c r="I19" s="22">
+        <f t="shared" ref="I19:L19" si="0">AVERAGE(I3:I6)</f>
+        <v>83.933813999999998</v>
+      </c>
+      <c r="J19" s="22">
+        <f t="shared" si="0"/>
+        <v>93.460095749999994</v>
+      </c>
+      <c r="K19" s="22">
+        <f t="shared" si="0"/>
+        <v>96.610876750000003</v>
+      </c>
+      <c r="L19" s="22">
+        <f t="shared" si="0"/>
+        <v>90.369458749999993</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F20" s="19"/>
+      <c r="G20" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="19">
+        <f>AVERAGE(H7:H10)</f>
+        <v>81.899825750000005</v>
+      </c>
+      <c r="I20" s="19">
+        <f t="shared" ref="I20:L20" si="1">AVERAGE(I7:I10)</f>
+        <v>83.15528574999999</v>
+      </c>
+      <c r="J20" s="19">
+        <f t="shared" si="1"/>
+        <v>87.133537750000002</v>
+      </c>
+      <c r="K20" s="19">
+        <f t="shared" si="1"/>
+        <v>92.718204750000012</v>
+      </c>
+      <c r="L20" s="19">
+        <f t="shared" si="1"/>
+        <v>81.418596500000007</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F21" s="19"/>
+      <c r="G21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="19">
+        <f>AVERAGE(H11:H14)</f>
+        <v>78.502001750000005</v>
+      </c>
+      <c r="I21" s="19">
+        <f t="shared" ref="I21:L21" si="2">AVERAGE(I11:I14)</f>
+        <v>81.636261500000003</v>
+      </c>
+      <c r="J21" s="19">
+        <f t="shared" si="2"/>
+        <v>73.462588750000009</v>
+      </c>
+      <c r="K21" s="19">
+        <f t="shared" si="2"/>
+        <v>84.319260499999999</v>
+      </c>
+      <c r="L21" s="19">
+        <f t="shared" si="2"/>
+        <v>62.778233499999999</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F22" s="19"/>
+      <c r="G22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="19">
+        <f>AVERAGE(H15:H17)</f>
+        <v>76.997209999999995</v>
+      </c>
+      <c r="I22" s="19">
+        <f t="shared" ref="I22:L22" si="3">AVERAGE(I15:I17)</f>
+        <v>81.027842666666672</v>
+      </c>
+      <c r="J22" s="19">
+        <f t="shared" si="3"/>
+        <v>66.164813333333328</v>
+      </c>
+      <c r="K22" s="19">
+        <f t="shared" si="3"/>
+        <v>81.133950666666664</v>
+      </c>
+      <c r="L22" s="19">
+        <f t="shared" si="3"/>
+        <v>53.526854666666672</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+    </row>
+    <row r="24" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="19">
+        <f>(H3*$E3+H4*$E4+H5*$E5+H6*$E6)/SUM($E3:$E6)</f>
+        <v>83.363065566268844</v>
+      </c>
+      <c r="I24" s="19">
+        <f t="shared" ref="I24:L24" si="4">(I3*$E3+I4*$E4+I5*$E5+I6*$E6)/SUM($E3:$E6)</f>
+        <v>83.964038979271365</v>
+      </c>
+      <c r="J24" s="19">
+        <f t="shared" si="4"/>
+        <v>93.702889438599229</v>
+      </c>
+      <c r="K24" s="19">
+        <f t="shared" si="4"/>
+        <v>96.686557860552767</v>
+      </c>
+      <c r="L24" s="19">
+        <f t="shared" si="4"/>
+        <v>90.640703603172099</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="F25" s="19"/>
+      <c r="G25" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="G26" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="G27" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:N17">
+    <sortCondition ref="M3:M17"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B17004E-B792-B74C-AB90-D27A5E2F8F4E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>